<commit_message>
user name and password changed
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>mngr83460</t>
-  </si>
-  <si>
-    <t>qAbUzyj</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -33,22 +28,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr112909</t>
+    <t>mngr429183</t>
   </si>
   <si>
-    <t>tytUreg</t>
-  </si>
-  <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
-  </si>
-  <si>
-    <t>mngr422789</t>
-  </si>
-  <si>
-    <t>zyhuguj</t>
+    <t>Avamyze</t>
   </si>
 </sst>
 </file>
@@ -441,7 +424,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,50 +435,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>